<commit_message>
dm/roundstart Init fixes and further testing
</commit_message>
<xml_diff>
--- a/z-options.xlsx
+++ b/z-options.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Code\Repos\Fantasy-Grounds\Extensions\AD-D-Options-and-House-Rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4003EB2B-1AC0-4434-9CBF-599933828792}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CD42934-460A-4BC5-B8C3-6D63E72B5DA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2115" yWindow="4845" windowWidth="31815" windowHeight="15480" xr2:uid="{E2C7049B-7416-4A2F-BFDC-166E242B304D}"/>
+    <workbookView xWindow="4890" yWindow="2910" windowWidth="29370" windowHeight="15480" xr2:uid="{E2C7049B-7416-4A2F-BFDC-166E242B304D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="79">
   <si>
     <t>Testing AD&amp;D Options and House Rules</t>
   </si>
@@ -67,9 +67,6 @@
     <t>X</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>Issues</t>
   </si>
   <si>
@@ -124,9 +121,6 @@
     <t>d6, no override</t>
   </si>
   <si>
-    <t>2e allow group ties = off doesn't prevent ties onroundstart</t>
-  </si>
-  <si>
     <t>X fix OSRIC using d6 only for init</t>
   </si>
   <si>
@@ -136,9 +130,6 @@
     <t>further checking onroundstart for all options in 2E and OSRIC</t>
   </si>
   <si>
-    <t>consider whether to dynamically display some options or leave a disclaimer under each one</t>
-  </si>
-  <si>
     <t>Damage: Critical Hit Type</t>
   </si>
   <si>
@@ -223,9 +214,6 @@
     <t>Ascending</t>
   </si>
   <si>
-    <t>test defaults again, matching spreadsheet</t>
-  </si>
-  <si>
     <t>1E</t>
   </si>
   <si>
@@ -266,16 +254,41 @@
   </si>
   <si>
     <t>no init mods, individual init, no swap</t>
+  </si>
+  <si>
+    <t>X test defaults again, matching spreadsheet</t>
+  </si>
+  <si>
+    <t>X consider whether to dynamically display some options or leave a disclaimer under each one</t>
+  </si>
+  <si>
+    <t>init drag no longer working</t>
+  </si>
+  <si>
+    <t>X 2e allow group ties = off doesn't prevent ties onroundstart</t>
+  </si>
+  <si>
+    <t>********2AM - 10/03 JUST OVERRODE getRoll</t>
+  </si>
+  <si>
+    <t>*** INIT BUTTON NOT WORKING IN OSRIC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -307,9 +320,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -624,15 +642,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{338CC476-3DB1-4186-AB3A-DA30E03453AC}">
-  <dimension ref="A1:F68"/>
+  <dimension ref="A1:F69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="35.7109375" customWidth="1"/>
+    <col min="1" max="1" width="43" customWidth="1"/>
+    <col min="2" max="2" width="35.7109375" customWidth="1"/>
     <col min="3" max="3" width="51.42578125" customWidth="1"/>
     <col min="4" max="4" width="21.7109375" customWidth="1"/>
     <col min="5" max="5" width="26.85546875" customWidth="1"/>
@@ -649,44 +668,44 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E3" t="s">
         <v>3</v>
       </c>
       <c r="F3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D5" t="s">
         <v>8</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -697,13 +716,13 @@
         <v>9</v>
       </c>
       <c r="D6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" t="s">
         <v>50</v>
-      </c>
-      <c r="E6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -711,7 +730,7 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D7" t="s">
         <v>8</v>
@@ -720,43 +739,49 @@
         <v>9</v>
       </c>
       <c r="F7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="C8" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="D8" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C9" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D9" t="s">
         <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C10" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D10" t="s">
         <v>8</v>
@@ -765,15 +790,15 @@
         <v>9</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C11" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D11" t="s">
         <v>8</v>
@@ -782,15 +807,15 @@
         <v>9</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C12" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D12" t="s">
         <v>8</v>
@@ -799,7 +824,7 @@
         <v>9</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -807,7 +832,7 @@
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D13" t="s">
         <v>8</v>
@@ -816,167 +841,167 @@
         <v>9</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C14" t="s">
         <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E14" t="s">
         <v>9</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C15" t="s">
         <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E15" t="s">
         <v>9</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C16" t="s">
         <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E16" t="s">
         <v>9</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C17" t="s">
         <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E17" t="s">
         <v>9</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C18" t="s">
         <v>9</v>
       </c>
       <c r="D18" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E18" t="s">
         <v>9</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D19" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D21" s="1">
+        <v>13</v>
+      </c>
+      <c r="D21" s="2">
         <v>-10</v>
       </c>
-      <c r="F21" s="1">
+      <c r="F21" s="2">
         <v>-10</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C23" t="s">
         <v>9</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E23" t="s">
         <v>9</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>8</v>
@@ -985,54 +1010,54 @@
         <v>9</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E25" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>8</v>
@@ -1041,79 +1066,79 @@
         <v>9</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C29" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E29" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>24</v>
+      </c>
+      <c r="C30" t="s">
         <v>25</v>
-      </c>
-      <c r="C30" t="s">
-        <v>26</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E30" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B38" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>29</v>
+        <v>76</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>31</v>
+        <v>75</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -1123,75 +1148,127 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B60" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
         <v>2</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C61" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>68</v>
-      </c>
-      <c r="B61" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B62" t="s">
-        <v>72</v>
+        <v>68</v>
+      </c>
+      <c r="C62" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="B63" t="s">
-        <v>72</v>
+        <v>68</v>
+      </c>
+      <c r="C63" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B64" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="C64" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>68</v>
+      </c>
+      <c r="C65" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>66</v>
+      </c>
+      <c r="B66" t="s">
+        <v>9</v>
+      </c>
+      <c r="C66" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>67</v>
+      </c>
+      <c r="B67" t="s">
+        <v>9</v>
+      </c>
+      <c r="C67" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>76</v>
+      <c r="B68" t="s">
+        <v>9</v>
+      </c>
+      <c r="C68" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>72</v>
+      </c>
+      <c r="B69" t="s">
+        <v>9</v>
+      </c>
+      <c r="C69" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Many changes, working through options and spreadsheet to make sure all possibilities work correctly
</commit_message>
<xml_diff>
--- a/z-options.xlsx
+++ b/z-options.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Code\Repos\Fantasy-Grounds\Extensions\AD-D-Options-and-House-Rules\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CD42934-460A-4BC5-B8C3-6D63E72B5DA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB36CC6C-E84E-4E4B-9D80-287808B68B63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4890" yWindow="2910" windowWidth="29370" windowHeight="15480" xr2:uid="{E2C7049B-7416-4A2F-BFDC-166E242B304D}"/>
+    <workbookView xWindow="2955" yWindow="3180" windowWidth="29265" windowHeight="15480" xr2:uid="{E2C7049B-7416-4A2F-BFDC-166E242B304D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="93">
   <si>
     <t>Testing AD&amp;D Options and House Rules</t>
   </si>
@@ -67,7 +67,7 @@
     <t>X</t>
   </si>
   <si>
-    <t>Issues</t>
+    <t>?</t>
   </si>
   <si>
     <t>X reset on round start = off causing all inits to be rolled in OSRIC</t>
@@ -100,9 +100,6 @@
     <t>Surprise: Die</t>
   </si>
   <si>
-    <t>2e init die change doesn't immediately take effect, not worrying about that right now</t>
-  </si>
-  <si>
     <t>NPC: Auto Hit Points</t>
   </si>
   <si>
@@ -127,9 +124,6 @@
     <t>X initiative grouping doesn't work onroundstart</t>
   </si>
   <si>
-    <t>further checking onroundstart for all options in 2E and OSRIC</t>
-  </si>
-  <si>
     <t>Damage: Critical Hit Type</t>
   </si>
   <si>
@@ -223,12 +217,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>TEST DM ROLLING INIT IN 2E (BROKEN)</t>
-  </si>
-  <si>
-    <t>consider option dependencies</t>
-  </si>
-  <si>
     <t>init mods, group init</t>
   </si>
   <si>
@@ -262,16 +250,70 @@
     <t>X consider whether to dynamically display some options or leave a disclaimer under each one</t>
   </si>
   <si>
-    <t>init drag no longer working</t>
-  </si>
-  <si>
     <t>X 2e allow group ties = off doesn't prevent ties onroundstart</t>
   </si>
   <si>
-    <t>********2AM - 10/03 JUST OVERRODE getRoll</t>
-  </si>
-  <si>
-    <t>*** INIT BUTTON NOT WORKING IN OSRIC</t>
+    <t>X init drag no longer working</t>
+  </si>
+  <si>
+    <t>X TEST DM ROLLING INIT IN 2E (BROKEN)</t>
+  </si>
+  <si>
+    <t>X 2e init die change doesn't immediately take effect, not worrying about that right now</t>
+  </si>
+  <si>
+    <t>X further checking onroundstart for all options in 2E and OSRIC</t>
+  </si>
+  <si>
+    <t>Critical Hit still displays on rolls of 20, regardless of options. Not worth it to bring in OnAttack right now</t>
+  </si>
+  <si>
+    <t>Death Effect doesn't get added to NPCs, but not really considering that necessary since they're dead at 0</t>
+  </si>
+  <si>
+    <t>Death for NPCs, regardless of option</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  off/0/-10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  off/-3/-10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  off/death-1/-10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  on/0/-10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  on/-3/-10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  on/death-1/-10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  on/0/-con</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  on/-3/-con</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  on/death-1/-con</t>
+  </si>
+  <si>
+    <t>ACCEPTED ISSUES</t>
+  </si>
+  <si>
+    <t>Discovered ISSUES</t>
+  </si>
+  <si>
+    <t>Deaths' Door PCs</t>
+  </si>
+  <si>
+    <t>X Advance round with bleeding character doesn't add dead</t>
+  </si>
+  <si>
+    <t>Advance round with bleeding character doesn't remove unconcious</t>
   </si>
 </sst>
 </file>
@@ -287,14 +329,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFC00000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -304,6 +347,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -320,14 +369,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -642,15 +692,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{338CC476-3DB1-4186-AB3A-DA30E03453AC}">
-  <dimension ref="A1:F69"/>
+  <dimension ref="A1:F71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43" customWidth="1"/>
+    <col min="1" max="1" width="88" customWidth="1"/>
     <col min="2" max="2" width="35.7109375" customWidth="1"/>
     <col min="3" max="3" width="51.42578125" customWidth="1"/>
     <col min="4" max="4" width="21.7109375" customWidth="1"/>
@@ -668,44 +718,44 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E3" t="s">
         <v>3</v>
       </c>
       <c r="F3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D5" t="s">
         <v>8</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -716,13 +766,13 @@
         <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E6" t="s">
         <v>9</v>
       </c>
       <c r="F6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -730,7 +780,7 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D7" t="s">
         <v>8</v>
@@ -739,7 +789,7 @@
         <v>9</v>
       </c>
       <c r="F7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -750,21 +800,21 @@
         <v>9</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D9" t="s">
         <v>8</v>
@@ -773,15 +823,15 @@
         <v>9</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D10" t="s">
         <v>8</v>
@@ -790,15 +840,15 @@
         <v>9</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D11" t="s">
         <v>8</v>
@@ -807,15 +857,15 @@
         <v>9</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C12" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D12" t="s">
         <v>8</v>
@@ -824,7 +874,7 @@
         <v>9</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -832,7 +882,7 @@
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D13" t="s">
         <v>8</v>
@@ -841,58 +891,58 @@
         <v>9</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C14" t="s">
         <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E14" t="s">
         <v>9</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C15" t="s">
         <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E15" t="s">
         <v>9</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C16" t="s">
         <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E16" t="s">
         <v>9</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -903,52 +953,55 @@
         <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E17" t="s">
         <v>9</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C18" t="s">
         <v>9</v>
       </c>
       <c r="D18" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E18" t="s">
         <v>9</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -967,16 +1020,16 @@
         <v>14</v>
       </c>
       <c r="C22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -987,13 +1040,13 @@
         <v>9</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E23" t="s">
         <v>9</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1001,7 +1054,7 @@
         <v>16</v>
       </c>
       <c r="C24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>8</v>
@@ -1010,7 +1063,7 @@
         <v>9</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1018,16 +1071,16 @@
         <v>17</v>
       </c>
       <c r="C25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1035,10 +1088,10 @@
         <v>18</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -1046,10 +1099,10 @@
         <v>19</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1057,7 +1110,7 @@
         <v>20</v>
       </c>
       <c r="C28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>8</v>
@@ -1066,205 +1119,298 @@
         <v>9</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C29" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E29" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>23</v>
+      </c>
+      <c r="C30" t="s">
         <v>24</v>
-      </c>
-      <c r="C30" t="s">
-        <v>25</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E30" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>78</v>
+      </c>
+      <c r="C34" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>79</v>
+      </c>
+      <c r="C36" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+      <c r="C37" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>81</v>
+      </c>
+      <c r="C38" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>82</v>
+      </c>
+      <c r="C39" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>83</v>
+      </c>
+      <c r="C40" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>84</v>
+      </c>
+      <c r="C41" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>60</v>
+      </c>
+      <c r="B46" t="s">
+        <v>64</v>
+      </c>
+      <c r="C46" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>61</v>
+      </c>
+      <c r="B47" t="s">
+        <v>64</v>
+      </c>
+      <c r="C47" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>65</v>
+      </c>
+      <c r="B48" t="s">
+        <v>64</v>
+      </c>
+      <c r="C48" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>66</v>
+      </c>
+      <c r="B49" t="s">
+        <v>64</v>
+      </c>
+      <c r="C49" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>62</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B50" t="s">
+        <v>9</v>
+      </c>
+      <c r="C50" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="B51" t="s">
+        <v>9</v>
+      </c>
+      <c r="C51" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>67</v>
+      </c>
+      <c r="B52" t="s">
+        <v>9</v>
+      </c>
+      <c r="C52" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>68</v>
+      </c>
+      <c r="B53" t="s">
+        <v>9</v>
+      </c>
+      <c r="C53" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="4" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B61" t="s">
-        <v>2</v>
-      </c>
-      <c r="C61" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>64</v>
-      </c>
-      <c r="B62" t="s">
-        <v>68</v>
-      </c>
-      <c r="C62" t="s">
-        <v>9</v>
+        <v>75</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>65</v>
-      </c>
-      <c r="B63" t="s">
-        <v>68</v>
-      </c>
-      <c r="C63" t="s">
-        <v>9</v>
+        <v>27</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>69</v>
       </c>
-      <c r="B64" t="s">
-        <v>68</v>
-      </c>
-      <c r="C64" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>70</v>
-      </c>
-      <c r="B65" t="s">
-        <v>68</v>
-      </c>
-      <c r="C65" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>66</v>
-      </c>
-      <c r="B66" t="s">
-        <v>9</v>
-      </c>
-      <c r="C66" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>67</v>
-      </c>
-      <c r="B67" t="s">
-        <v>9</v>
-      </c>
-      <c r="C67" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>71</v>
-      </c>
-      <c r="B68" t="s">
-        <v>9</v>
-      </c>
-      <c r="C68" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>72</v>
-      </c>
-      <c r="B69" t="s">
-        <v>9</v>
-      </c>
-      <c r="C69" t="s">
-        <v>9</v>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>